<commit_message>
Se agrega lo conversado en cada ceremonia
</commit_message>
<xml_diff>
--- a/Daily.xlsx
+++ b/Daily.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24603"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fi365-my.sharepoint.com/personal/df201671_fi365_ort_edu_uy/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{163CF8A8-4955-403E-B469-AC65C10C20A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="567" documentId="8_{778C0240-FE77-40D4-AE62-B7858F471A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83379D3B-4840-4952-A71B-26C17D2CD32B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteración 1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="89">
   <si>
     <t>Semana 1</t>
   </si>
@@ -182,6 +182,103 @@
     <t>Semana 4</t>
   </si>
   <si>
+    <t>Martes 5/10</t>
+  </si>
+  <si>
+    <t>jueves 7/10</t>
+  </si>
+  <si>
+    <t>viernes 8/10</t>
+  </si>
+  <si>
+    <t>sábado 9/10</t>
+  </si>
+  <si>
+    <t>lunes 11/10</t>
+  </si>
+  <si>
+    <t>miércoles 13/10</t>
+  </si>
+  <si>
+    <t>viernes 15/10</t>
+  </si>
+  <si>
+    <t>domingo 17/10</t>
+  </si>
+  <si>
+    <t>Se realizo un estudio de diseño para la protipacion de las interfaces de usuario. En este punto se estudian 6 fases para lograr la correcta prototipacion.
+Se definieron las historias que se van a incluir en este sprint con sus narrativas y criterios de aceptación.</t>
+  </si>
+  <si>
+    <t>Estoy trabajando en completmentar la documentación con el estudio de diseño para la prototipación.</t>
+  </si>
+  <si>
+    <t>Sigo trabjando en la documentación. Voy a justificar el uso de las herramientas elegidas.</t>
+  </si>
+  <si>
+    <t>Voy a revisar la interfaz de métricas. Estoy escribiendo el feedback.</t>
+  </si>
+  <si>
+    <t>Voy a revisar la interfaz de alertas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voy a incorporar los prints de la evolución a la documentación. </t>
+  </si>
+  <si>
+    <t>Se evaluaron los resultados del Sprint 2. 
+Se validaron todas las tareas completadas.
+Se compartieron los prototipos generados y se explicaron las funcionalidades consideradas.
+Se validaron los prototipos con el usuario y se recogió feedback para implementar en la siguiente iteración.</t>
+  </si>
+  <si>
+    <t>Estoy comenzando con el diseño de la interfaz de dosis restantes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigo trabajando en el diseño de la interfaz de dosis restantes. Voy a trabajar en emprolijar los departamentos. </t>
+  </si>
+  <si>
+    <t>Terminé con el diseño de interfaz de dosis restantes.
+Voy a revisando la interfaz de home.</t>
+  </si>
+  <si>
+    <t>Voy a incorporar el feedback recibido de la interfaz de diagnóstico y de métricas.</t>
+  </si>
+  <si>
+    <t>Voy a revisar la interfaz de alertas y hacer las modificaciones necesarias.</t>
+  </si>
+  <si>
+    <t>Estoy comenzando con el diseño de la interfaz de métricas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigo trabajando en el diseño de la interfaz de métricas. </t>
+  </si>
+  <si>
+    <t>Terminé con el diseño de interfaz de métricas.
+Estoy trabajando en la documentación sobre el mapa de empatía.</t>
+  </si>
+  <si>
+    <t>Voy a incorporar el feedback recibido de la interfaz de home.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Voy a incorporar el feedback recibido de la interfaz de dosis restantes</t>
+  </si>
+  <si>
+    <t>Estoy comenzando con el diseño de la interfaz de diagnóstico.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigo trabajando en el diseño de la interfaz de diagnóstico, tuve dificultades para los efectos de transiciones y tuve que ponerme a investigar. </t>
+  </si>
+  <si>
+    <t>Terminé con el diseño de interfaz de diagnóstico.
+Voy a revisar la interfaz de  dosis restantes.</t>
+  </si>
+  <si>
+    <t>Terminé de revisar la interfaz de dosis restantes y sigo con la de diagnóstico.</t>
+  </si>
+  <si>
+    <t>Estoy revisando la interfaz de diagnósitco con el feedback recibido.</t>
+  </si>
+  <si>
     <t>Semana 5</t>
   </si>
   <si>
@@ -207,13 +304,39 @@
   </si>
   <si>
     <t>Daily (Viernes 01/10)</t>
+  </si>
+  <si>
+    <t>Sprint Planning
+I2</t>
+  </si>
+  <si>
+    <t>Daily (Jueves 7/10)</t>
+  </si>
+  <si>
+    <t>Daily (Viernes 8/10)</t>
+  </si>
+  <si>
+    <t>Daily (Sabado 9/10)</t>
+  </si>
+  <si>
+    <t>Daily (Lunes 11/10)</t>
+  </si>
+  <si>
+    <t>Daily (Miercoles 13/10)</t>
+  </si>
+  <si>
+    <t>Sprint Review (Viernes 15/10)</t>
+  </si>
+  <si>
+    <t>Para el siguiente Sprint pensamos continuar con el mismo ritmo de trabajo.
+En este segundo Sprint ya tenemos más experiencia que en el anterior para calcular los SP de cada historia. También pudimos calcular con cuidado las dependencias de cada tarea por lo que pusimos fechas límites para las primeras tareas para que se puedan completar las siguientes. Seguiremos utilizando las mismas herramientas elegidas más Framer que nos resultó muy útil.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -263,6 +386,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -470,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -536,6 +666,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -894,6 +1027,356 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>258</xdr:row>
+      <xdr:rowOff>82627</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BD0BED9-EB8D-400B-BF47-0DDA5055389C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="35318700"/>
+          <a:ext cx="12058650" cy="7858202"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>8465</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>157693</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>429865</xdr:colOff>
+      <xdr:row>306</xdr:row>
+      <xdr:rowOff>37043</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EF940D4-6468-4097-9F02-3B2330FB715D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="651932" y="43278426"/>
+          <a:ext cx="12003800" cy="7327900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>14350</xdr:colOff>
+      <xdr:row>358</xdr:row>
+      <xdr:rowOff>14350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>493362</xdr:colOff>
+      <xdr:row>404</xdr:row>
+      <xdr:rowOff>130919</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B7BB095-A586-40F3-8A85-9846856C2B38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="660113" y="57874689"/>
+          <a:ext cx="12061412" cy="7565119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>309</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>411875</xdr:colOff>
+      <xdr:row>354</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86FCA5C3-E3C5-473B-8A43-01A0464E2DE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="51349275"/>
+          <a:ext cx="11997450" cy="7327900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>408</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>339725</xdr:colOff>
+      <xdr:row>459</xdr:row>
+      <xdr:rowOff>102887</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E969AF80-CF32-471B-AFB8-1BE6AD26C609}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="67379850"/>
+          <a:ext cx="11922125" cy="8364237"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>32609</xdr:colOff>
+      <xdr:row>463</xdr:row>
+      <xdr:rowOff>7175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>281258</xdr:colOff>
+      <xdr:row>519</xdr:row>
+      <xdr:rowOff>16123</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C641FA9-35A4-43D3-B33E-7D4D3170D937}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="796675" y="77714655"/>
+          <a:ext cx="11831049" cy="9076748"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>521</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>291583</xdr:colOff>
+      <xdr:row>577</xdr:row>
+      <xdr:rowOff>121432</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88E75E69-A0C9-4D62-8524-B90C6CDA3408}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="764066" y="87289269"/>
+          <a:ext cx="11873983" cy="9274956"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1100,41 +1583,41 @@
   </sheetPr>
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="F5" workbookViewId="0">
       <selection activeCell="I4" sqref="I4:I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" style="2" customWidth="1"/>
     <col min="4" max="4" width="39" style="2" customWidth="1"/>
     <col min="5" max="5" width="28" style="2" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.26953125" style="2" customWidth="1"/>
     <col min="7" max="7" width="30" style="2" customWidth="1"/>
-    <col min="8" max="8" width="31.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="31.26953125" style="2" customWidth="1"/>
     <col min="9" max="9" width="29" style="2" customWidth="1"/>
-    <col min="16384" max="16384" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16384" max="16384" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" ht="50.1" customHeight="1">
+    <row r="1" spans="1:19" s="3" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="14"/>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="32" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="13"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:19" s="3" customFormat="1" ht="50.1" customHeight="1">
+    <row r="2" spans="1:19" s="3" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
@@ -1164,7 +1647,7 @@
       </c>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:19" s="3" customFormat="1" ht="50.1" customHeight="1">
+    <row r="3" spans="1:19" s="3" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>8</v>
@@ -1201,14 +1684,14 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" s="3" customFormat="1" ht="65.25" customHeight="1">
+    <row r="4" spans="1:19" s="3" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -1223,19 +1706,19 @@
       <c r="G4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="3" customFormat="1" ht="66" customHeight="1">
+    <row r="5" spans="1:19" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="10" t="s">
         <v>26</v>
       </c>
@@ -1248,15 +1731,15 @@
       <c r="G5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="27"/>
-      <c r="I5" s="30"/>
-    </row>
-    <row r="6" spans="1:19" s="3" customFormat="1" ht="64.5" customHeight="1">
+      <c r="H5" s="28"/>
+      <c r="I5" s="31"/>
+    </row>
+    <row r="6" spans="1:19" s="3" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="10" t="s">
         <v>31</v>
       </c>
@@ -1269,15 +1752,15 @@
       <c r="G6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="30"/>
-    </row>
-    <row r="7" spans="1:19" s="3" customFormat="1" ht="77.25" customHeight="1">
+      <c r="H6" s="28"/>
+      <c r="I6" s="31"/>
+    </row>
+    <row r="7" spans="1:19" s="3" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="10" t="s">
         <v>36</v>
       </c>
@@ -1290,8 +1773,8 @@
       <c r="G7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="31"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1317,133 +1800,211 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F75200F-7A6C-426A-948D-F53BF09095AF}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="11" width="15.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.26953125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="35.26953125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="40.26953125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="50.1" customHeight="1">
+    <row r="1" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-    </row>
-    <row r="2" spans="1:11" ht="50.1" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9">
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+    </row>
+    <row r="2" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9">
-        <v>3</v>
-      </c>
-      <c r="E2" s="9">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9">
+      <c r="C2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="8">
-        <v>1</v>
-      </c>
-      <c r="H2" s="8">
-        <v>2</v>
-      </c>
-      <c r="I2" s="8">
-        <v>3</v>
-      </c>
-      <c r="J2" s="8">
-        <v>4</v>
-      </c>
-      <c r="K2" s="8">
+      <c r="D2" s="23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="50.1" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="E2" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" spans="1:11" ht="50.1" customHeight="1">
-      <c r="A4" s="12" t="s">
+      <c r="B4" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="11"/>
-    </row>
-    <row r="5" spans="1:11" ht="50.1" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="28"/>
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="6" spans="1:11" ht="50.1" customHeight="1">
-      <c r="A6" s="12" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="28"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="11"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="29"/>
+      <c r="I7" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" location="Trello!A211" display="Sprint planning" xr:uid="{2672FF1E-89E3-4A18-975F-EF89346E26A3}"/>
+    <hyperlink ref="C2" location="Trello!A262" display="Daily meeting" xr:uid="{FA68DE8A-E689-4ED2-98F6-20F039335458}"/>
+    <hyperlink ref="D2" location="Trello!A310" display="Daily meeting" xr:uid="{7210FBD4-D508-4F1A-8285-D010790A000C}"/>
+    <hyperlink ref="E2" location="Trello!A359" display="Daily meeting" xr:uid="{35A51A9B-A3E0-46F7-97CC-3077520AF829}"/>
+    <hyperlink ref="F2" location="Trello!A409" display="Daily meeting" xr:uid="{67C419DB-7A60-4B2B-B98C-B750133B2D42}"/>
+    <hyperlink ref="G2" location="Trello!A464" display="Daily meeting" xr:uid="{19C6E31F-EFFC-439D-BD36-0EDF99608B3F}"/>
+    <hyperlink ref="H2" location="Trello!A522" display="Sprint review" xr:uid="{2B859CA1-F1CA-45F0-BAF4-27ACD375C6F9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1456,30 +2017,30 @@
       <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="15.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="15.7265625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="50.1" customHeight="1">
+    <row r="1" spans="1:11" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
-      <c r="B1" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-    </row>
-    <row r="2" spans="1:11" ht="50.1" customHeight="1">
+      <c r="B1" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+    </row>
+    <row r="2" spans="1:11" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8">
         <v>1</v>
@@ -1512,7 +2073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="50.1" customHeight="1">
+    <row r="3" spans="1:11" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
@@ -1527,7 +2088,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:11" ht="50.1" customHeight="1">
+    <row r="4" spans="1:11" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>25</v>
       </c>
@@ -1542,7 +2103,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" ht="50.1" customHeight="1">
+    <row r="5" spans="1:11" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>30</v>
       </c>
@@ -1557,7 +2118,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:11" ht="50.1" customHeight="1">
+    <row r="6" spans="1:11" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>35</v>
       </c>
@@ -1589,30 +2150,30 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="15.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="15.7265625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="50.1" customHeight="1">
+    <row r="1" spans="1:11" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
-      <c r="B1" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-    </row>
-    <row r="2" spans="1:11" ht="50.1" customHeight="1">
+      <c r="B1" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+    </row>
+    <row r="2" spans="1:11" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8">
         <v>1</v>
@@ -1645,7 +2206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="50.1" customHeight="1">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
@@ -1660,7 +2221,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="50.1" customHeight="1">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>25</v>
       </c>
@@ -1675,7 +2236,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="50.1" customHeight="1">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>30</v>
       </c>
@@ -1690,7 +2251,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="50.1" customHeight="1">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>35</v>
       </c>
@@ -1716,100 +2277,208 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7D779E-1B89-42A6-8B48-E575D427ACB5}">
-  <dimension ref="A1:A176"/>
+  <dimension ref="A1:A525"/>
   <sheetViews>
     <sheetView topLeftCell="A133" workbookViewId="0">
       <selection activeCell="A173" sqref="A173:A176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="28.5" customHeight="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A2" s="40"/>
-    </row>
-    <row r="3" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A3" s="40"/>
-    </row>
-    <row r="4" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A4" s="41"/>
-    </row>
-    <row r="28" spans="1:1" ht="57" customHeight="1">
-      <c r="A28" s="39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A29" s="40"/>
-    </row>
-    <row r="30" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A30" s="40"/>
-    </row>
-    <row r="31" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A31" s="41"/>
-    </row>
-    <row r="67" spans="1:1" ht="42.75" customHeight="1">
-      <c r="A67" s="39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A68" s="40"/>
-    </row>
-    <row r="69" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A69" s="40"/>
-    </row>
-    <row r="70" spans="1:1" ht="14.25" customHeight="1">
-      <c r="A70" s="41"/>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="39" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" s="40"/>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107" s="40"/>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" s="41"/>
-    </row>
-    <row r="138" spans="1:1">
-      <c r="A138" s="39" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1">
-      <c r="A139" s="40"/>
-    </row>
-    <row r="140" spans="1:1">
-      <c r="A140" s="40"/>
-    </row>
-    <row r="141" spans="1:1">
-      <c r="A141" s="41"/>
-    </row>
-    <row r="173" spans="1:1">
-      <c r="A173" s="39" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1">
-      <c r="A174" s="40"/>
-    </row>
-    <row r="175" spans="1:1">
-      <c r="A175" s="40"/>
-    </row>
-    <row r="176" spans="1:1">
-      <c r="A176" s="41"/>
+    <row r="2" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="41"/>
+    </row>
+    <row r="3" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+    </row>
+    <row r="4" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="42"/>
+    </row>
+    <row r="28" spans="1:1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="41"/>
+    </row>
+    <row r="30" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="41"/>
+    </row>
+    <row r="31" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="42"/>
+    </row>
+    <row r="67" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="41"/>
+    </row>
+    <row r="69" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="41"/>
+    </row>
+    <row r="70" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="42"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="41"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="41"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="42"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="41"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="41"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="42"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="41"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="41"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="42"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="41"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="41"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="42"/>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="41"/>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="41"/>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="42"/>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="41"/>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="41"/>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="42"/>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="41"/>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="41"/>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="42"/>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="41"/>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="41"/>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" s="42"/>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="41"/>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="41"/>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="42"/>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" s="40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" s="41"/>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" s="41"/>
+    </row>
+    <row r="525" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A525" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="13">
+    <mergeCell ref="A464:A467"/>
+    <mergeCell ref="A522:A525"/>
+    <mergeCell ref="A211:A214"/>
+    <mergeCell ref="A262:A265"/>
+    <mergeCell ref="A310:A313"/>
+    <mergeCell ref="A359:A362"/>
+    <mergeCell ref="A409:A412"/>
     <mergeCell ref="A138:A141"/>
     <mergeCell ref="A173:A176"/>
     <mergeCell ref="A1:A4"/>
@@ -2061,13 +2730,45 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEED0ADC-9893-4498-BBB0-0E59F240259A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEED0ADC-9893-4498-BBB0-0E59F240259A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="017fa494-680b-4af0-b2e3-750edd48b64a"/>
+    <ds:schemaRef ds:uri="83a202e8-1e8b-4917-a92b-945fd3882671"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B52DFA0B-57FF-4123-AD29-7430B14998F4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B52DFA0B-57FF-4123-AD29-7430B14998F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="017fa494-680b-4af0-b2e3-750edd48b64a"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="83a202e8-1e8b-4917-a92b-945fd3882671"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D90DEEAE-27E1-4C32-BA1D-D1ECB4840F59}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D90DEEAE-27E1-4C32-BA1D-D1ECB4840F59}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>